<commit_message>
Fixed several errors with comparison and filling of numeric types. POI can be a pain sometimes (we know to blame Microsoft though).
</commit_message>
<xml_diff>
--- a/samples/sample_input.xlsx
+++ b/samples/sample_input.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>InputInt1</t>
   </si>
@@ -41,6 +41,12 @@
     <t>OutputDec1</t>
   </si>
   <si>
+    <t>AutoFill1</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
     <t>Hello</t>
   </si>
   <si>
@@ -71,16 +77,13 @@
     <t>buzz</t>
   </si>
   <si>
-    <t>aWrongVal</t>
-  </si>
-  <si>
     <t>a string</t>
   </si>
   <si>
-    <t>another wrong</t>
-  </si>
-  <si>
     <t>EnumVal11</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -155,11 +158,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,10 +180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -223,6 +222,9 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -234,14 +236,14 @@
       <c r="C2" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1.1</v>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -261,10 +263,10 @@
         <v>2.22</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>4</v>
@@ -284,10 +286,10 @@
         <v>3.333</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0</v>
@@ -307,10 +309,10 @@
         <v>4.4444</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>4</v>
@@ -327,10 +329,10 @@
         <v>5.55555</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>20</v>
@@ -347,10 +349,10 @@
         <v>6.666666</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>30</v>
@@ -367,13 +369,13 @@
         <v>7.7777777</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,9 +389,9 @@
         <v>8.8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -423,6 +425,11 @@
       </c>
       <c r="D11" s="0" t="n">
         <v>10.101010101</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>